<commit_message>
JEYZ-69 : Open file descriptor monitoring rules added
</commit_message>
<xml_diff>
--- a/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
+++ b/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\jeyzer\analyzer\src\main\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\jeyzer\jeyzer-analyzer\analyzer\src\main\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42214F1D-6420-4267-AADF-2DEB462D7712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9D5D5A-C367-47D5-BB5F-1B2DAE3DE004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20268" yWindow="252" windowWidth="20376" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event params logged" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="200">
   <si>
     <t>END DATE</t>
   </si>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <t>pattern + signal</t>
+  </si>
+  <si>
+    <t>Open file descriptor number</t>
+  </si>
+  <si>
+    <t>Open file descriptor percentage</t>
   </si>
 </sst>
 </file>
@@ -1199,13 +1205,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z93"/>
+  <dimension ref="A1:Z95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J80" sqref="J80"/>
+      <selection pane="bottomRight" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2920,220 +2926,215 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>71</v>
+        <v>199</v>
       </c>
       <c r="B53" s="8">
         <v>2</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="C53" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J53" t="s">
         <v>27</v>
       </c>
       <c r="N53" s="1"/>
-      <c r="O53" s="7">
-        <v>1</v>
-      </c>
+      <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
-      <c r="S53" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T53">
-        <v>1</v>
-      </c>
-      <c r="V53" t="s">
-        <v>23</v>
-      </c>
+      <c r="S53" s="1"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>120</v>
+        <v>198</v>
       </c>
       <c r="B54" s="8">
         <v>2</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="C54" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J54" t="s">
         <v>27</v>
       </c>
       <c r="N54" s="1"/>
-      <c r="O54" s="7">
-        <v>1</v>
-      </c>
+      <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
-      <c r="S54" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T54">
-        <v>1</v>
-      </c>
-      <c r="V54" t="s">
-        <v>23</v>
-      </c>
+      <c r="S54" s="1"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B55" s="8">
         <v>2</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F55" s="8" t="s">
+      <c r="D55" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J55" t="s">
-        <v>35</v>
-      </c>
-      <c r="M55" s="1"/>
+        <v>27</v>
+      </c>
       <c r="N55" s="1"/>
-      <c r="O55" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P55" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="O55" s="7">
+        <v>1</v>
+      </c>
+      <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
-      <c r="S55" s="1"/>
+      <c r="S55" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T55">
         <v>1</v>
       </c>
-      <c r="U55" t="s">
-        <v>88</v>
+      <c r="V55" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="B56" s="8">
-        <v>1</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="G56" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J56" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M56" s="1"/>
-      <c r="O56" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J56" t="s">
+        <v>27</v>
+      </c>
+      <c r="N56" s="1"/>
+      <c r="O56" s="7">
+        <v>1</v>
+      </c>
+      <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
+      <c r="S56" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T56">
-        <v>2</v>
-      </c>
-      <c r="U56" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="V56" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B57" s="8">
-        <v>1</v>
-      </c>
-      <c r="D57" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J57" t="s">
-        <v>44</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="O57" s="7">
-        <v>1</v>
-      </c>
-      <c r="P57" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57">
         <v>1</v>
       </c>
+      <c r="U57" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B58" s="8">
         <v>1</v>
       </c>
       <c r="C58" s="8"/>
-      <c r="D58" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J58" t="s">
-        <v>44</v>
-      </c>
-      <c r="K58" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O58" s="7">
-        <v>1</v>
-      </c>
-      <c r="P58" s="1"/>
+      <c r="D58" s="8"/>
+      <c r="G58" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J58" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M58" s="1"/>
+      <c r="O58" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="U58" t="s">
+        <v>113</v>
+      </c>
+      <c r="V58" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B59" s="8">
         <v>1</v>
       </c>
-      <c r="C59" s="8"/>
       <c r="D59" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J59" t="s">
-        <v>27</v>
-      </c>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="O59" s="7">
+        <v>1</v>
+      </c>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
-      <c r="S59" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S59" s="1"/>
       <c r="T59">
-        <v>2</v>
-      </c>
-      <c r="V59" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B60" s="8">
         <v>1</v>
@@ -3143,9 +3144,11 @@
         <v>46</v>
       </c>
       <c r="J60" t="s">
-        <v>34</v>
-      </c>
-      <c r="M60" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="O60" s="7">
         <v>1</v>
       </c>
@@ -3153,18 +3156,15 @@
       <c r="Q60" s="1"/>
       <c r="S60" s="1"/>
       <c r="T60">
-        <v>2</v>
-      </c>
-      <c r="V60" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>164</v>
+        <v>68</v>
       </c>
       <c r="B61" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8" t="s">
@@ -3174,24 +3174,22 @@
         <v>27</v>
       </c>
       <c r="N61" s="1"/>
-      <c r="O61" s="7">
-        <v>1</v>
-      </c>
+      <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="S61" s="1" t="s">
         <v>46</v>
       </c>
       <c r="T61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V61" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B62" s="8">
         <v>1</v>
@@ -3201,11 +3199,9 @@
         <v>46</v>
       </c>
       <c r="J62" t="s">
-        <v>44</v>
-      </c>
-      <c r="K62" s="6" t="s">
-        <v>80</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M62" s="1"/>
       <c r="O62" s="7">
         <v>1</v>
       </c>
@@ -3213,40 +3209,45 @@
       <c r="Q62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="V62" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="B63" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J63" t="s">
-        <v>34</v>
-      </c>
-      <c r="M63" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N63" s="1"/>
       <c r="O63" s="7">
         <v>1</v>
       </c>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
-      <c r="S63" s="1"/>
+      <c r="S63" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T63">
         <v>1</v>
       </c>
       <c r="V63" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B64" s="8">
         <v>1</v>
@@ -3256,27 +3257,24 @@
         <v>46</v>
       </c>
       <c r="J64" t="s">
-        <v>27</v>
-      </c>
-      <c r="N64" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="O64" s="7">
         <v>1</v>
       </c>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="S64" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S64" s="1"/>
       <c r="T64">
         <v>1</v>
-      </c>
-      <c r="V64" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B65" s="8">
         <v>1</v>
@@ -3304,55 +3302,49 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="B66" s="8">
-        <v>4</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F66" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J66" t="s">
-        <v>148</v>
-      </c>
-      <c r="K66" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N66" s="6" t="s">
-        <v>149</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N66" s="1"/>
       <c r="O66" s="7">
         <v>1</v>
       </c>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
-      <c r="S66" s="1"/>
+      <c r="S66" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
       <c r="V66" t="s">
-        <v>150</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
-        <v>179</v>
+        <v>78</v>
       </c>
       <c r="B67" s="8">
-        <v>2</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C67" s="8"/>
       <c r="D67" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J67" t="s">
-        <v>44</v>
-      </c>
-      <c r="K67" s="6" t="s">
-        <v>180</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M67" s="1"/>
       <c r="O67" s="7">
         <v>1</v>
       </c>
@@ -3362,25 +3354,31 @@
       <c r="T67">
         <v>1</v>
       </c>
+      <c r="V67" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="B68" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="F68" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J68" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="K68" s="6" t="s">
-        <v>177</v>
+        <v>53</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="O68" s="7">
         <v>1</v>
@@ -3388,16 +3386,16 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="S68" s="1"/>
-      <c r="T68">
-        <v>1</v>
+      <c r="V68" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B69" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>46</v>
@@ -3406,9 +3404,11 @@
         <v>46</v>
       </c>
       <c r="J69" t="s">
-        <v>34</v>
-      </c>
-      <c r="M69" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="O69" s="7">
         <v>1</v>
       </c>
@@ -3418,16 +3418,13 @@
       <c r="T69">
         <v>1</v>
       </c>
-      <c r="U69" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B70" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>46</v>
@@ -3436,9 +3433,11 @@
         <v>46</v>
       </c>
       <c r="J70" t="s">
-        <v>34</v>
-      </c>
-      <c r="M70" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>177</v>
+      </c>
       <c r="O70" s="7">
         <v>1</v>
       </c>
@@ -3448,13 +3447,10 @@
       <c r="T70">
         <v>1</v>
       </c>
-      <c r="U70" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B71" s="8">
         <v>1</v>
@@ -3466,11 +3462,9 @@
         <v>46</v>
       </c>
       <c r="J71" t="s">
-        <v>44</v>
-      </c>
-      <c r="K71" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M71" s="1"/>
       <c r="O71" s="7">
         <v>1</v>
       </c>
@@ -3486,7 +3480,7 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B72" s="8">
         <v>1</v>
@@ -3498,11 +3492,9 @@
         <v>46</v>
       </c>
       <c r="J72" t="s">
-        <v>44</v>
-      </c>
-      <c r="K72" s="6" t="s">
-        <v>176</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M72" s="1"/>
       <c r="O72" s="7">
         <v>1</v>
       </c>
@@ -3512,13 +3504,16 @@
       <c r="T72">
         <v>1</v>
       </c>
+      <c r="U72" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B73" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>46</v>
@@ -3530,7 +3525,7 @@
         <v>44</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="O73" s="7">
         <v>1</v>
@@ -3541,10 +3536,13 @@
       <c r="T73">
         <v>1</v>
       </c>
+      <c r="U73" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B74" s="8">
         <v>1</v>
@@ -3556,9 +3554,11 @@
         <v>46</v>
       </c>
       <c r="J74" t="s">
-        <v>34</v>
-      </c>
-      <c r="M74" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="O74" s="7">
         <v>1</v>
       </c>
@@ -3568,16 +3568,13 @@
       <c r="T74">
         <v>1</v>
       </c>
-      <c r="U74" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B75" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>46</v>
@@ -3586,9 +3583,11 @@
         <v>46</v>
       </c>
       <c r="J75" t="s">
-        <v>34</v>
-      </c>
-      <c r="M75" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="O75" s="7">
         <v>1</v>
       </c>
@@ -3598,13 +3597,10 @@
       <c r="T75">
         <v>1</v>
       </c>
-      <c r="U75" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B76" s="8">
         <v>1</v>
@@ -3616,11 +3612,9 @@
         <v>46</v>
       </c>
       <c r="J76" t="s">
-        <v>44</v>
-      </c>
-      <c r="K76" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M76" s="1"/>
       <c r="O76" s="7">
         <v>1</v>
       </c>
@@ -3636,7 +3630,7 @@
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B77" s="8">
         <v>1</v>
@@ -3648,11 +3642,9 @@
         <v>46</v>
       </c>
       <c r="J77" t="s">
-        <v>44</v>
-      </c>
-      <c r="K77" s="6" t="s">
-        <v>185</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M77" s="1"/>
       <c r="O77" s="7">
         <v>1</v>
       </c>
@@ -3662,13 +3654,16 @@
       <c r="T77">
         <v>1</v>
       </c>
+      <c r="U77" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B78" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>46</v>
@@ -3680,7 +3675,7 @@
         <v>44</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="O78" s="7">
         <v>1</v>
@@ -3691,26 +3686,32 @@
       <c r="T78">
         <v>1</v>
       </c>
+      <c r="U78" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="B79" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D79" s="8"/>
-      <c r="F79" s="8" t="s">
+      <c r="D79" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J79" t="s">
-        <v>27</v>
-      </c>
-      <c r="N79" s="1"/>
-      <c r="O79"/>
+        <v>44</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="O79" s="7">
+        <v>1</v>
+      </c>
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
       <c r="S79" s="1"/>
@@ -3720,19 +3721,22 @@
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B80" s="8">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J80" t="s">
-        <v>197</v>
+        <v>44</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="O80" s="7">
         <v>1</v>
@@ -3740,19 +3744,22 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
       <c r="S80" s="1"/>
-      <c r="U80" t="s">
-        <v>88</v>
+      <c r="T80">
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="B81" s="8">
-        <v>1</v>
-      </c>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D81" s="8"/>
+      <c r="F81" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J81" t="s">
@@ -3762,245 +3769,228 @@
       <c r="O81"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
-      <c r="S81" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S81" s="1"/>
       <c r="T81">
         <v>1</v>
-      </c>
-      <c r="U81" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="B82" s="8">
-        <v>2</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F82" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J82" t="s">
-        <v>27</v>
-      </c>
-      <c r="N82" s="1"/>
-      <c r="O82" s="6" t="s">
-        <v>31</v>
+        <v>197</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="O82" s="7">
+        <v>1</v>
       </c>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
       <c r="S82" s="1"/>
-      <c r="T82">
-        <v>1</v>
-      </c>
-      <c r="V82" t="s">
-        <v>63</v>
+      <c r="U82" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="B83" s="8">
-        <v>4</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D83" s="8"/>
-      <c r="F83" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J83" t="s">
-        <v>44</v>
-      </c>
-      <c r="K83" s="6" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="N83" s="1"/>
-      <c r="O83" s="7">
-        <v>1</v>
-      </c>
+      <c r="O83"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
-      <c r="S83" s="1"/>
+      <c r="S83" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T83">
+        <v>1</v>
+      </c>
+      <c r="U83" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>156</v>
-      </c>
-      <c r="B84">
-        <v>1</v>
-      </c>
+      <c r="A84" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="8">
+        <v>2</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D84" s="8"/>
       <c r="E84" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F84" t="s">
-        <v>46</v>
-      </c>
-      <c r="J84" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M84" s="1"/>
+      <c r="F84" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J84" t="s">
+        <v>27</v>
+      </c>
+      <c r="N84" s="1"/>
       <c r="O84" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P84" s="2"/>
-      <c r="Q84" t="s">
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="T84">
+        <v>1</v>
+      </c>
+      <c r="V84" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A85" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" s="8">
+        <v>4</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D85" s="8"/>
+      <c r="F85" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J85" t="s">
+        <v>44</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N85" s="1"/>
+      <c r="O85" s="7">
+        <v>1</v>
+      </c>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="S85" s="1"/>
+      <c r="W85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>156</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F86" t="s">
+        <v>46</v>
+      </c>
+      <c r="J86" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M86" s="1"/>
+      <c r="O86" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P86" s="2"/>
+      <c r="Q86" t="s">
         <v>3</v>
       </c>
-      <c r="T84">
-        <v>1</v>
-      </c>
-      <c r="U84" t="s">
-        <v>88</v>
-      </c>
-      <c r="V84" t="s">
-        <v>11</v>
-      </c>
-      <c r="W84" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85">
-        <v>4</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H85" t="s">
-        <v>46</v>
-      </c>
-      <c r="J85" t="s">
-        <v>27</v>
-      </c>
-      <c r="N85" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O85" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P85" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q85" s="1"/>
-      <c r="R85" s="1"/>
-      <c r="S85" s="1"/>
-      <c r="T85">
-        <v>1</v>
-      </c>
-      <c r="U85" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A86" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B86" s="8">
-        <v>1</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G86" s="8"/>
-      <c r="J86" t="s">
-        <v>44</v>
-      </c>
-      <c r="K86" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="O86" s="7">
-        <v>1</v>
-      </c>
-      <c r="P86" s="1"/>
-      <c r="Q86" s="1"/>
-      <c r="R86" s="1"/>
-      <c r="S86" s="1"/>
       <c r="T86">
         <v>1</v>
       </c>
       <c r="U86" t="s">
         <v>88</v>
       </c>
+      <c r="V86" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A87" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B87" s="8">
-        <v>5</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F87" s="8" t="s">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87">
+        <v>4</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H87" t="s">
         <v>46</v>
       </c>
       <c r="J87" t="s">
-        <v>44</v>
-      </c>
-      <c r="K87" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="O87" s="7">
-        <v>1</v>
-      </c>
-      <c r="P87" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O87" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P87" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
       <c r="S87" s="1"/>
       <c r="T87">
         <v>1</v>
       </c>
-      <c r="V87" t="s">
-        <v>167</v>
+      <c r="U87" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
       <c r="B88" s="8">
-        <v>4</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F88" s="8" t="s">
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G88" s="8"/>
       <c r="J88" t="s">
-        <v>27</v>
-      </c>
-      <c r="N88" s="1"/>
-      <c r="O88" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="O88" s="7">
+        <v>1</v>
       </c>
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
       <c r="S88" s="1"/>
       <c r="T88">
         <v>1</v>
       </c>
-      <c r="V88" t="s">
-        <v>14</v>
+      <c r="U88" t="s">
+        <v>88</v>
       </c>
       <c r="Y88" s="8" t="s">
         <v>47</v>
@@ -4011,105 +4001,83 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="B89" s="8">
-        <v>1</v>
-      </c>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="G89" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H89" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J89" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L89" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M89" s="1"/>
-      <c r="O89" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P89" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J89" t="s">
+        <v>44</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="O89" s="7">
+        <v>1</v>
+      </c>
+      <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
-      <c r="R89" s="1"/>
       <c r="S89" s="1"/>
       <c r="T89">
         <v>1</v>
       </c>
-      <c r="U89" t="s">
-        <v>87</v>
+      <c r="V89" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>155</v>
-      </c>
-      <c r="B90">
-        <v>1</v>
-      </c>
-      <c r="C90" t="s">
-        <v>46</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H90" t="s">
+      <c r="A90" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" s="8">
+        <v>4</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F90" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J90" t="s">
         <v>27</v>
-      </c>
-      <c r="L90" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="N90" s="1"/>
       <c r="O90" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P90" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
-      <c r="S90" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S90" s="1"/>
       <c r="T90">
         <v>1</v>
       </c>
-      <c r="U90" t="s">
-        <v>87</v>
-      </c>
       <c r="V90" t="s">
-        <v>23</v>
-      </c>
-      <c r="W90" t="s">
-        <v>24</v>
-      </c>
-      <c r="X90" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>116</v>
-      </c>
-      <c r="B91">
-        <v>1</v>
-      </c>
-      <c r="C91" t="s">
-        <v>46</v>
-      </c>
+      <c r="A91" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B91" s="8">
+        <v>1</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
       <c r="G91" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J91" s="10" t="s">
@@ -4126,6 +4094,7 @@
         <v>4</v>
       </c>
       <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
       <c r="S91" s="1"/>
       <c r="T91">
         <v>1</v>
@@ -4133,9 +4102,6 @@
       <c r="U91" t="s">
         <v>87</v>
       </c>
-      <c r="V91" t="s">
-        <v>27</v>
-      </c>
       <c r="W91" t="s">
         <v>24</v>
       </c>
@@ -4145,53 +4111,143 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="B92">
         <v>1</v>
       </c>
-      <c r="I92" t="s">
+      <c r="C92" t="s">
+        <v>46</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H92" t="s">
         <v>46</v>
       </c>
       <c r="J92" t="s">
-        <v>44</v>
-      </c>
-      <c r="K92" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="O92" s="7">
-        <v>1</v>
-      </c>
-      <c r="P92" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="L92" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N92" s="1"/>
+      <c r="O92" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P92" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q92" s="1"/>
-      <c r="S92" s="1"/>
+      <c r="S92" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T92">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="U92" t="s">
+        <v>87</v>
+      </c>
+      <c r="V92" t="s">
+        <v>23</v>
+      </c>
+      <c r="W92" t="s">
+        <v>24</v>
+      </c>
+      <c r="X92" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
-      <c r="I93" t="s">
-        <v>46</v>
-      </c>
-      <c r="J93" t="s">
-        <v>44</v>
-      </c>
-      <c r="K93" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="O93" s="7">
-        <v>1</v>
-      </c>
-      <c r="P93" s="1"/>
+      <c r="C93" t="s">
+        <v>46</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H93" t="s">
+        <v>46</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L93" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M93" s="1"/>
+      <c r="O93" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P93" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q93" s="1"/>
       <c r="S93" s="1"/>
       <c r="T93">
+        <v>1</v>
+      </c>
+      <c r="U93" t="s">
+        <v>87</v>
+      </c>
+      <c r="V93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="I94" t="s">
+        <v>46</v>
+      </c>
+      <c r="J94" t="s">
+        <v>44</v>
+      </c>
+      <c r="K94" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O94" s="7">
+        <v>1</v>
+      </c>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="I95" t="s">
+        <v>46</v>
+      </c>
+      <c r="J95" t="s">
+        <v>44</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O95" s="7">
+        <v>1</v>
+      </c>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
JEYZ-72 : Shared profile monitoring rule support
</commit_message>
<xml_diff>
--- a/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
+++ b/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\jeyzer\jeyzer-analyzer\analyzer\src\main\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9D5D5A-C367-47D5-BB5F-1B2DAE3DE004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B559C800-CCD1-43AC-9808-F8EF277610E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20268" yWindow="252" windowWidth="20376" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event params logged" sheetId="1" r:id="rId1"/>
     <sheet name="Level colors" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event params logged'!$A$1:$Z$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event params logged'!$A$1:$Z$94</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="202">
   <si>
     <t>END DATE</t>
   </si>
@@ -646,6 +646,12 @@
   </si>
   <si>
     <t>Open file descriptor percentage</t>
+  </si>
+  <si>
+    <t>Shared profile</t>
+  </si>
+  <si>
+    <t>shared profile</t>
   </si>
 </sst>
 </file>
@@ -1205,13 +1211,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z95"/>
+  <dimension ref="A1:Z96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomRight" activeCell="T86" sqref="T86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3917,6 +3923,7 @@
       <c r="Q86" t="s">
         <v>3</v>
       </c>
+      <c r="S86" s="1"/>
       <c r="T86">
         <v>1</v>
       </c>
@@ -3928,61 +3935,54 @@
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="A87" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B87" s="8">
+        <v>1</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E87" s="8"/>
+      <c r="J87" t="s">
+        <v>44</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="O87" s="6"/>
+      <c r="P87" s="2"/>
+      <c r="S87" s="1"/>
+      <c r="V87" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>6</v>
       </c>
-      <c r="B87">
+      <c r="B88">
         <v>4</v>
       </c>
-      <c r="G87" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H87" t="s">
-        <v>46</v>
-      </c>
-      <c r="J87" t="s">
+      <c r="G88" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H88" t="s">
+        <v>46</v>
+      </c>
+      <c r="J88" t="s">
         <v>27</v>
       </c>
-      <c r="N87" s="1" t="s">
+      <c r="N88" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O87" s="6" t="s">
+      <c r="O88" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P87" s="1" t="s">
+      <c r="P88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q87" s="1"/>
-      <c r="R87" s="1"/>
-      <c r="S87" s="1"/>
-      <c r="T87">
-        <v>1</v>
-      </c>
-      <c r="U87" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A88" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B88" s="8">
-        <v>1</v>
-      </c>
-      <c r="D88" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G88" s="8"/>
-      <c r="J88" t="s">
-        <v>44</v>
-      </c>
-      <c r="K88" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="O88" s="7">
-        <v>1</v>
-      </c>
-      <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
@@ -3990,58 +3990,53 @@
         <v>1</v>
       </c>
       <c r="U88" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y88" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z88" s="8" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B89" s="8">
-        <v>5</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G89" s="8"/>
       <c r="J89" t="s">
         <v>44</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="O89" s="7">
         <v>1</v>
       </c>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
       <c r="S89" s="1"/>
       <c r="T89">
         <v>1</v>
       </c>
-      <c r="V89" t="s">
-        <v>167</v>
+      <c r="U89" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y89" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z89" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="B90" s="8">
-        <v>4</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D90" s="8"/>
+        <v>5</v>
+      </c>
       <c r="E90" s="8" t="s">
         <v>46</v>
       </c>
@@ -4049,11 +4044,13 @@
         <v>46</v>
       </c>
       <c r="J90" t="s">
-        <v>27</v>
-      </c>
-      <c r="N90" s="1"/>
-      <c r="O90" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="K90" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="O90" s="7">
+        <v>1</v>
       </c>
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
@@ -4062,76 +4059,65 @@
         <v>1</v>
       </c>
       <c r="V90" t="s">
-        <v>14</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B91" s="8">
-        <v>1</v>
-      </c>
-      <c r="C91" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D91" s="8"/>
-      <c r="G91" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H91" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J91" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L91" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M91" s="1"/>
+      <c r="E91" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F91" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J91" t="s">
+        <v>27</v>
+      </c>
+      <c r="N91" s="1"/>
       <c r="O91" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P91" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
-      <c r="R91" s="1"/>
       <c r="S91" s="1"/>
       <c r="T91">
         <v>1</v>
       </c>
-      <c r="U91" t="s">
-        <v>87</v>
-      </c>
-      <c r="W91" t="s">
-        <v>24</v>
-      </c>
-      <c r="X91" t="s">
-        <v>26</v>
+      <c r="V91" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>155</v>
-      </c>
-      <c r="B92">
-        <v>1</v>
-      </c>
-      <c r="C92" t="s">
-        <v>46</v>
-      </c>
+      <c r="A92" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B92" s="8">
+        <v>1</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
       <c r="G92" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H92" t="s">
-        <v>46</v>
-      </c>
-      <c r="J92" t="s">
-        <v>27</v>
+      <c r="H92" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J92" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="L92" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N92" s="1"/>
+      <c r="M92" s="1"/>
       <c r="O92" s="6" t="s">
         <v>31</v>
       </c>
@@ -4139,18 +4125,14 @@
         <v>4</v>
       </c>
       <c r="Q92" s="1"/>
-      <c r="S92" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
       <c r="T92">
         <v>1</v>
       </c>
       <c r="U92" t="s">
         <v>87</v>
       </c>
-      <c r="V92" t="s">
-        <v>23</v>
-      </c>
       <c r="W92" t="s">
         <v>24</v>
       </c>
@@ -4160,7 +4142,7 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -4174,13 +4156,13 @@
       <c r="H93" t="s">
         <v>46</v>
       </c>
-      <c r="J93" s="10" t="s">
-        <v>34</v>
+      <c r="J93" t="s">
+        <v>27</v>
       </c>
       <c r="L93" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
       <c r="O93" s="6" t="s">
         <v>31</v>
       </c>
@@ -4188,7 +4170,9 @@
         <v>4</v>
       </c>
       <c r="Q93" s="1"/>
-      <c r="S93" s="1"/>
+      <c r="S93" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T93">
         <v>1</v>
       </c>
@@ -4196,38 +4180,59 @@
         <v>87</v>
       </c>
       <c r="V93" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="W93" t="s">
+        <v>24</v>
+      </c>
+      <c r="X93" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
-      <c r="I94" t="s">
-        <v>46</v>
-      </c>
-      <c r="J94" t="s">
-        <v>44</v>
-      </c>
-      <c r="K94" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="O94" s="7">
-        <v>1</v>
-      </c>
-      <c r="P94" s="1"/>
+      <c r="C94" t="s">
+        <v>46</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H94" t="s">
+        <v>46</v>
+      </c>
+      <c r="J94" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L94" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M94" s="1"/>
+      <c r="O94" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P94" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q94" s="1"/>
       <c r="S94" s="1"/>
       <c r="T94">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="U94" t="s">
+        <v>87</v>
+      </c>
+      <c r="V94" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -4239,7 +4244,7 @@
         <v>44</v>
       </c>
       <c r="K95" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O95" s="7">
         <v>1</v>
@@ -4251,10 +4256,36 @@
         <v>0</v>
       </c>
     </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="I96" t="s">
+        <v>46</v>
+      </c>
+      <c r="J96" t="s">
+        <v>44</v>
+      </c>
+      <c r="K96" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O96" s="7">
+        <v>1</v>
+      </c>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Z93" xr:uid="{32A5E267-3EA0-4E71-9FF7-CDD296A6772F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z93">
-      <sortCondition ref="A1:A92"/>
+  <autoFilter ref="A1:Z94" xr:uid="{32A5E267-3EA0-4E71-9FF7-CDD296A6772F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z94">
+      <sortCondition ref="A1:A93"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
JEYZ-82 : Executor presence monitoring rule
</commit_message>
<xml_diff>
--- a/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
+++ b/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\jeyzer\jeyzer-analyzer\analyzer\src\main\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E953366-8F67-4C86-B969-387F40208A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3758A7DD-0899-4A79-98F8-68F9E3D217ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Level colors" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event params logged'!$A$1:$Z$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event params logged'!$A$1:$Z$95</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="204">
   <si>
     <t>END DATE</t>
   </si>
@@ -652,6 +652,12 @@
   </si>
   <si>
     <t>shared profile</t>
+  </si>
+  <si>
+    <t>Executor presence</t>
+  </si>
+  <si>
+    <t>Executor detected</t>
   </si>
 </sst>
 </file>
@@ -891,9 +897,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -931,9 +937,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -966,26 +972,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1018,26 +1007,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1211,13 +1183,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z96"/>
+  <dimension ref="A1:Z97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T87" sqref="T87"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2066,106 +2038,105 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="A26" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J26" t="s">
         <v>44</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O26" s="6"/>
-      <c r="P26" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="N26" s="1"/>
+      <c r="O26" s="7">
+        <v>1</v>
+      </c>
+      <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26">
-        <v>2</v>
-      </c>
-      <c r="U26" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B27" s="8">
-        <v>2</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="8" t="s">
+      <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" t="s">
         <v>46</v>
       </c>
       <c r="J27" t="s">
-        <v>129</v>
-      </c>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="O27" s="6"/>
       <c r="P27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>70</v>
+        <v>157</v>
       </c>
       <c r="B28" s="8">
         <v>2</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J28" t="s">
-        <v>27</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="7">
-        <v>1</v>
-      </c>
-      <c r="P28" s="1"/>
+      <c r="O28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q28" s="1"/>
-      <c r="S28" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S28" s="1"/>
       <c r="T28">
         <v>1</v>
       </c>
-      <c r="V28" t="s">
-        <v>23</v>
+      <c r="U28" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="B29" s="8">
         <v>2</v>
@@ -2194,59 +2165,51 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B30" s="8">
         <v>2</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J30" t="s">
-        <v>35</v>
-      </c>
-      <c r="M30" s="1"/>
+        <v>27</v>
+      </c>
       <c r="N30" s="1"/>
-      <c r="O30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="O30" s="7">
+        <v>1</v>
+      </c>
+      <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="S30" s="1"/>
+      <c r="S30" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T30">
         <v>1</v>
       </c>
-      <c r="U30" t="s">
-        <v>88</v>
+      <c r="V30" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B31" s="8">
-        <v>1</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="G31" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" t="s">
+        <v>35</v>
       </c>
       <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
       <c r="O31" s="6" t="s">
         <v>31</v>
       </c>
@@ -2254,47 +2217,58 @@
         <v>4</v>
       </c>
       <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U31" t="s">
-        <v>112</v>
-      </c>
-      <c r="V31" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B32" s="8">
         <v>1</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J32" t="s">
-        <v>44</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="O32" s="7">
-        <v>1</v>
-      </c>
-      <c r="P32" s="1"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="G32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M32" s="1"/>
+      <c r="O32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="U32" t="s">
+        <v>112</v>
+      </c>
+      <c r="V32" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="B33" s="8">
         <v>1</v>
@@ -2302,177 +2276,170 @@
       <c r="D33" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J33" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M33" s="1"/>
+      <c r="J33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="O33" s="7">
+        <v>1</v>
+      </c>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33">
         <v>1</v>
       </c>
-      <c r="U33" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" t="s">
-        <v>46</v>
-      </c>
-      <c r="J34" t="s">
-        <v>62</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O34" s="1"/>
+      <c r="A34" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34">
         <v>1</v>
       </c>
-      <c r="V34" t="s">
-        <v>17</v>
+      <c r="U34" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35" s="8">
-        <v>4</v>
-      </c>
-      <c r="F35" s="8" t="s">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" t="s">
         <v>46</v>
       </c>
       <c r="J35" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35">
         <v>1</v>
       </c>
       <c r="V35" t="s">
-        <v>110</v>
-      </c>
-      <c r="W35" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36">
+      <c r="A36" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="8">
         <v>4</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="F36" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J36" t="s">
-        <v>27</v>
-      </c>
-      <c r="N36" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="O36" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P36" s="1"/>
+      <c r="P36" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36">
         <v>1</v>
       </c>
       <c r="V36" t="s">
-        <v>14</v>
+        <v>110</v>
+      </c>
+      <c r="W36" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" s="8">
-        <v>1</v>
+      <c r="A37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" t="s">
         <v>46</v>
       </c>
       <c r="J37" t="s">
         <v>27</v>
       </c>
       <c r="N37" s="1"/>
-      <c r="O37" s="7">
-        <v>1</v>
+      <c r="O37" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="S37" s="1"/>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="V37" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>154</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>46</v>
+      <c r="A38" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="8">
+        <v>1</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J38" t="s">
         <v>27</v>
       </c>
       <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
+      <c r="O38" s="7">
+        <v>1</v>
+      </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
-      <c r="S38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T38">
-        <v>1</v>
-      </c>
-      <c r="V38" t="s">
-        <v>23</v>
-      </c>
+      <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2487,193 +2454,195 @@
         <v>46</v>
       </c>
       <c r="J39" t="s">
-        <v>34</v>
-      </c>
-      <c r="M39" s="1"/>
-      <c r="O39" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
-      <c r="S39" s="1"/>
+      <c r="S39" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T39">
         <v>1</v>
       </c>
       <c r="V39" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F40" s="8" t="s">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
         <v>46</v>
       </c>
       <c r="J40" t="s">
-        <v>145</v>
-      </c>
-      <c r="O40" s="7">
-        <v>1</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>146</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="O40" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40">
         <v>1</v>
       </c>
+      <c r="V40" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="A41" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O41" s="6"/>
+        <v>145</v>
+      </c>
+      <c r="O41" s="7">
+        <v>1</v>
+      </c>
       <c r="P41" s="1" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41">
         <v>1</v>
       </c>
-      <c r="U41" t="s">
-        <v>87</v>
-      </c>
-      <c r="V41" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="8">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42">
         <v>2</v>
       </c>
-      <c r="E42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="8" t="s">
+      <c r="G42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" t="s">
         <v>46</v>
       </c>
       <c r="J42" t="s">
-        <v>27</v>
-      </c>
-      <c r="N42" s="1"/>
-      <c r="O42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P42" s="1"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42">
         <v>1</v>
       </c>
+      <c r="U42" t="s">
+        <v>87</v>
+      </c>
       <c r="V42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="8">
         <v>2</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="E43" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J43" t="s">
-        <v>61</v>
-      </c>
-      <c r="L43" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43" s="1"/>
+      <c r="O43" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O43" s="6"/>
-      <c r="P43" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43">
-        <v>2</v>
-      </c>
-      <c r="U43" t="s">
-        <v>87</v>
+        <v>1</v>
+      </c>
+      <c r="V43" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F44" t="s">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
         <v>46</v>
       </c>
       <c r="J44" t="s">
-        <v>27</v>
-      </c>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O44" s="6"/>
+      <c r="P44" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44">
-        <v>1</v>
-      </c>
-      <c r="V44" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="U44" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="8">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
         <v>3</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" t="s">
         <v>46</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" t="s">
         <v>46</v>
       </c>
       <c r="J45" t="s">
@@ -2688,147 +2657,144 @@
         <v>1</v>
       </c>
       <c r="V45" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46">
-        <v>2</v>
-      </c>
-      <c r="C46" t="s">
-        <v>46</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H46" t="s">
+      <c r="A46" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="8">
+        <v>3</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J46" t="s">
         <v>27</v>
       </c>
-      <c r="L46" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="N46" s="1"/>
-      <c r="O46" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46">
         <v>1</v>
       </c>
-      <c r="U46" t="s">
-        <v>87</v>
-      </c>
       <c r="V46" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>46</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H47" t="s">
+        <v>46</v>
+      </c>
+      <c r="J47" t="s">
+        <v>27</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N47" s="1"/>
+      <c r="O47" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="U47" t="s">
+        <v>87</v>
+      </c>
+      <c r="V47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>168</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>3</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F47" t="s">
-        <v>46</v>
-      </c>
-      <c r="J47" t="s">
+      <c r="E48" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>46</v>
+      </c>
+      <c r="J48" t="s">
         <v>51</v>
       </c>
-      <c r="K47" s="6" t="s">
+      <c r="K48" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="O47" s="1" t="s">
+      <c r="O48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="S47" s="1"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B48" s="8">
-        <v>2</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J48" t="s">
-        <v>114</v>
-      </c>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="S48" s="1"/>
-      <c r="T48">
-        <v>1</v>
-      </c>
-      <c r="U48" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B49" s="8">
-        <v>1</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="8"/>
+        <v>2</v>
+      </c>
       <c r="E49" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J49" t="s">
-        <v>27</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
+      <c r="O49" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q49" s="1"/>
-      <c r="S49" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S49" s="1"/>
       <c r="T49">
-        <v>2</v>
-      </c>
-      <c r="V49" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="U49" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="B50" s="8">
         <v>1</v>
@@ -2843,78 +2809,73 @@
       <c r="F50" t="s">
         <v>46</v>
       </c>
-      <c r="J50" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M50" s="1"/>
-      <c r="O50" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="J50" t="s">
+        <v>27</v>
+      </c>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
-      <c r="S50" s="1"/>
+      <c r="S50" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V50" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="B51" s="8">
-        <v>4</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J51" t="s">
-        <v>106</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" t="s">
+        <v>46</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M51" s="1"/>
       <c r="O51" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P51" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51">
         <v>1</v>
       </c>
-      <c r="U51" t="s">
-        <v>88</v>
-      </c>
       <c r="V51" t="s">
-        <v>110</v>
-      </c>
-      <c r="W51" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="B52" s="8">
-        <v>3</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J52" t="s">
-        <v>35</v>
-      </c>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="O52" s="6" t="s">
         <v>31</v>
       </c>
@@ -2924,21 +2885,24 @@
       <c r="Q52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U52" t="s">
         <v>88</v>
       </c>
+      <c r="V52" t="s">
+        <v>110</v>
+      </c>
+      <c r="W52" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="B53" s="8">
-        <v>2</v>
-      </c>
-      <c r="C53" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>46</v>
@@ -2947,17 +2911,28 @@
         <v>46</v>
       </c>
       <c r="J53" t="s">
-        <v>27</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="M53" s="1"/>
       <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
+      <c r="O53" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q53" s="1"/>
       <c r="S53" s="1"/>
+      <c r="T53">
+        <v>2</v>
+      </c>
+      <c r="U53" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B54" s="8">
         <v>2</v>
@@ -2982,36 +2957,32 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>71</v>
+        <v>198</v>
       </c>
       <c r="B55" s="8">
         <v>2</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="C55" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J55" t="s">
         <v>27</v>
       </c>
       <c r="N55" s="1"/>
-      <c r="O55" s="7">
-        <v>1</v>
-      </c>
+      <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
-      <c r="S55" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T55">
-        <v>1</v>
-      </c>
-      <c r="V55" t="s">
-        <v>23</v>
-      </c>
+      <c r="S55" s="1"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B56" s="8">
         <v>2</v>
@@ -3040,59 +3011,51 @@
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="B57" s="8">
         <v>2</v>
       </c>
-      <c r="E57" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F57" s="8" t="s">
+      <c r="D57" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J57" t="s">
-        <v>35</v>
-      </c>
-      <c r="M57" s="1"/>
+        <v>27</v>
+      </c>
       <c r="N57" s="1"/>
-      <c r="O57" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="O57" s="7">
+        <v>1</v>
+      </c>
+      <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
-      <c r="S57" s="1"/>
+      <c r="S57" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T57">
         <v>1</v>
       </c>
-      <c r="U57" t="s">
-        <v>88</v>
+      <c r="V57" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B58" s="8">
-        <v>1</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="G58" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J58" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J58" t="s">
+        <v>35</v>
       </c>
       <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
       <c r="O58" s="6" t="s">
         <v>31</v>
       </c>
@@ -3100,52 +3063,62 @@
         <v>4</v>
       </c>
       <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U58" t="s">
-        <v>113</v>
-      </c>
-      <c r="V58" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B59" s="8">
         <v>1</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J59" t="s">
-        <v>44</v>
-      </c>
-      <c r="K59" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="O59" s="7">
-        <v>1</v>
-      </c>
-      <c r="P59" s="1"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="G59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J59" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M59" s="1"/>
+      <c r="O59" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="U59" t="s">
+        <v>113</v>
+      </c>
+      <c r="V59" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="B60" s="8">
         <v>1</v>
       </c>
-      <c r="C60" s="8"/>
       <c r="D60" s="8" t="s">
         <v>46</v>
       </c>
@@ -3153,7 +3126,7 @@
         <v>44</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="O60" s="7">
         <v>1</v>
@@ -3167,7 +3140,7 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B61" s="8">
         <v>1</v>
@@ -3177,25 +3150,24 @@
         <v>46</v>
       </c>
       <c r="J61" t="s">
-        <v>27</v>
-      </c>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O61" s="7">
+        <v>1</v>
+      </c>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
-      <c r="S61" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S61" s="1"/>
       <c r="T61">
-        <v>2</v>
-      </c>
-      <c r="V61" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B62" s="8">
         <v>1</v>
@@ -3205,82 +3177,83 @@
         <v>46</v>
       </c>
       <c r="J62" t="s">
-        <v>34</v>
-      </c>
-      <c r="M62" s="1"/>
-      <c r="O62" s="7">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-      <c r="S62" s="1"/>
+      <c r="S62" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T62">
         <v>2</v>
       </c>
       <c r="V62" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
-        <v>164</v>
+        <v>66</v>
       </c>
       <c r="B63" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J63" t="s">
-        <v>27</v>
-      </c>
-      <c r="N63" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="M63" s="1"/>
       <c r="O63" s="7">
         <v>1</v>
       </c>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
-      <c r="S63" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S63" s="1"/>
       <c r="T63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V63" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B64" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J64" t="s">
-        <v>44</v>
-      </c>
-      <c r="K64" s="6" t="s">
-        <v>80</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N64" s="1"/>
       <c r="O64" s="7">
         <v>1</v>
       </c>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="S64" s="1"/>
+      <c r="S64" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T64">
         <v>1</v>
+      </c>
+      <c r="V64" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B65" s="8">
         <v>1</v>
@@ -3290,9 +3263,11 @@
         <v>46</v>
       </c>
       <c r="J65" t="s">
-        <v>34</v>
-      </c>
-      <c r="M65" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="O65" s="7">
         <v>1</v>
       </c>
@@ -3302,13 +3277,10 @@
       <c r="T65">
         <v>1</v>
       </c>
-      <c r="V65" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B66" s="8">
         <v>1</v>
@@ -3318,27 +3290,25 @@
         <v>46</v>
       </c>
       <c r="J66" t="s">
-        <v>27</v>
-      </c>
-      <c r="N66" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="M66" s="1"/>
       <c r="O66" s="7">
         <v>1</v>
       </c>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
-      <c r="S66" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S66" s="1"/>
       <c r="T66">
         <v>1</v>
       </c>
       <c r="V66" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" s="8">
         <v>1</v>
@@ -3348,72 +3318,73 @@
         <v>46</v>
       </c>
       <c r="J67" t="s">
-        <v>34</v>
-      </c>
-      <c r="M67" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N67" s="1"/>
       <c r="O67" s="7">
         <v>1</v>
       </c>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
-      <c r="S67" s="1"/>
+      <c r="S67" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T67">
         <v>1</v>
       </c>
       <c r="V67" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="B68" s="8">
-        <v>4</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F68" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J68" t="s">
-        <v>148</v>
-      </c>
-      <c r="K68" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N68" s="6" t="s">
-        <v>149</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M68" s="1"/>
       <c r="O68" s="7">
         <v>1</v>
       </c>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="S68" s="1"/>
+      <c r="T68">
+        <v>1</v>
+      </c>
       <c r="V68" t="s">
-        <v>150</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="B69" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="F69" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J69" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>180</v>
+        <v>53</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="O69" s="7">
         <v>1</v>
@@ -3421,16 +3392,16 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
       <c r="S69" s="1"/>
-      <c r="T69">
-        <v>1</v>
+      <c r="V69" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B70" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>46</v>
@@ -3442,7 +3413,7 @@
         <v>44</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="O70" s="7">
         <v>1</v>
@@ -3456,10 +3427,10 @@
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B71" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>46</v>
@@ -3468,9 +3439,11 @@
         <v>46</v>
       </c>
       <c r="J71" t="s">
-        <v>34</v>
-      </c>
-      <c r="M71" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>177</v>
+      </c>
       <c r="O71" s="7">
         <v>1</v>
       </c>
@@ -3480,13 +3453,10 @@
       <c r="T71">
         <v>1</v>
       </c>
-      <c r="U71" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B72" s="8">
         <v>1</v>
@@ -3516,7 +3486,7 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B73" s="8">
         <v>1</v>
@@ -3528,11 +3498,9 @@
         <v>46</v>
       </c>
       <c r="J73" t="s">
-        <v>44</v>
-      </c>
-      <c r="K73" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M73" s="1"/>
       <c r="O73" s="7">
         <v>1</v>
       </c>
@@ -3548,7 +3516,7 @@
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B74" s="8">
         <v>1</v>
@@ -3563,7 +3531,7 @@
         <v>44</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O74" s="7">
         <v>1</v>
@@ -3574,13 +3542,16 @@
       <c r="T74">
         <v>1</v>
       </c>
+      <c r="U74" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B75" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>46</v>
@@ -3592,7 +3563,7 @@
         <v>44</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O75" s="7">
         <v>1</v>
@@ -3606,10 +3577,10 @@
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B76" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>46</v>
@@ -3618,9 +3589,11 @@
         <v>46</v>
       </c>
       <c r="J76" t="s">
-        <v>34</v>
-      </c>
-      <c r="M76" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="O76" s="7">
         <v>1</v>
       </c>
@@ -3630,13 +3603,10 @@
       <c r="T76">
         <v>1</v>
       </c>
-      <c r="U76" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B77" s="8">
         <v>1</v>
@@ -3666,7 +3636,7 @@
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B78" s="8">
         <v>1</v>
@@ -3678,11 +3648,9 @@
         <v>46</v>
       </c>
       <c r="J78" t="s">
-        <v>44</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M78" s="1"/>
       <c r="O78" s="7">
         <v>1</v>
       </c>
@@ -3698,7 +3666,7 @@
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B79" s="8">
         <v>1</v>
@@ -3713,7 +3681,7 @@
         <v>44</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="O79" s="7">
         <v>1</v>
@@ -3724,13 +3692,16 @@
       <c r="T79">
         <v>1</v>
       </c>
+      <c r="U79" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B80" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>46</v>
@@ -3742,7 +3713,7 @@
         <v>44</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O80" s="7">
         <v>1</v>
@@ -3756,23 +3727,26 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="B81" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D81" s="8"/>
-      <c r="F81" s="8" t="s">
+      <c r="D81" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J81" t="s">
-        <v>27</v>
-      </c>
-      <c r="N81" s="1"/>
-      <c r="O81"/>
+        <v>44</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="O81" s="7">
+        <v>1</v>
+      </c>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
       <c r="S81" s="1"/>
@@ -3782,241 +3756,236 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="B82" s="8">
-        <v>5</v>
-      </c>
-      <c r="D82" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D82" s="8"/>
+      <c r="F82" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J82" t="s">
-        <v>197</v>
-      </c>
-      <c r="K82" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="O82" s="7">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N82" s="1"/>
+      <c r="O82"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
       <c r="S82" s="1"/>
-      <c r="U82" t="s">
-        <v>88</v>
+      <c r="T82">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B83" s="8">
-        <v>1</v>
-      </c>
-      <c r="C83" s="8"/>
+        <v>5</v>
+      </c>
       <c r="D83" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J83" t="s">
-        <v>27</v>
-      </c>
-      <c r="N83" s="1"/>
-      <c r="O83"/>
+        <v>197</v>
+      </c>
+      <c r="K83" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="O83" s="7">
+        <v>1</v>
+      </c>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
-      <c r="S83" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T83">
-        <v>1</v>
-      </c>
+      <c r="S83" s="1"/>
       <c r="U83" t="s">
-        <v>190</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="B84" s="8">
-        <v>2</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F84" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J84" t="s">
         <v>27</v>
       </c>
       <c r="N84" s="1"/>
-      <c r="O84" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="O84"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
-      <c r="S84" s="1"/>
+      <c r="S84" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T84">
         <v>1</v>
       </c>
-      <c r="V84" t="s">
-        <v>63</v>
+      <c r="U84" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="B85" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D85" s="8"/>
+      <c r="E85" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="F85" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J85" t="s">
-        <v>44</v>
-      </c>
-      <c r="K85" s="6" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="N85" s="1"/>
-      <c r="O85" s="7">
-        <v>1</v>
+      <c r="O85" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
       <c r="S85" s="1"/>
-      <c r="W85" t="s">
+      <c r="T85">
+        <v>1</v>
+      </c>
+      <c r="V85" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A86" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="8">
+        <v>4</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D86" s="8"/>
+      <c r="F86" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J86" t="s">
+        <v>44</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N86" s="1"/>
+      <c r="O86" s="7">
+        <v>1</v>
+      </c>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="W86" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>156</v>
       </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F86" t="s">
-        <v>46</v>
-      </c>
-      <c r="J86" s="10" t="s">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F87" t="s">
+        <v>46</v>
+      </c>
+      <c r="J87" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M86" s="1"/>
-      <c r="O86" s="6" t="s">
+      <c r="M87" s="1"/>
+      <c r="O87" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P86" s="2"/>
-      <c r="Q86" t="s">
+      <c r="P87" s="2"/>
+      <c r="Q87" t="s">
         <v>3</v>
       </c>
-      <c r="S86" s="1"/>
-      <c r="T86">
-        <v>1</v>
-      </c>
-      <c r="U86" t="s">
-        <v>88</v>
-      </c>
-      <c r="V86" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A87" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B87" s="8">
-        <v>1</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E87" s="8"/>
-      <c r="J87" t="s">
-        <v>44</v>
-      </c>
-      <c r="K87" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="O87" s="6"/>
-      <c r="P87" s="2"/>
       <c r="S87" s="1"/>
       <c r="T87">
         <v>1</v>
       </c>
+      <c r="U87" t="s">
+        <v>88</v>
+      </c>
       <c r="V87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A88" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B88" s="8">
+        <v>1</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E88" s="8"/>
+      <c r="J88" t="s">
+        <v>44</v>
+      </c>
+      <c r="K88" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>6</v>
-      </c>
-      <c r="B88">
-        <v>4</v>
-      </c>
-      <c r="G88" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H88" t="s">
-        <v>46</v>
-      </c>
-      <c r="J88" t="s">
-        <v>27</v>
-      </c>
-      <c r="N88" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O88" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P88" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q88" s="1"/>
-      <c r="R88" s="1"/>
+      <c r="O88" s="6"/>
+      <c r="P88" s="2"/>
       <c r="S88" s="1"/>
       <c r="T88">
         <v>1</v>
       </c>
-      <c r="U88" t="s">
-        <v>87</v>
+      <c r="V88" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A89" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B89" s="8">
-        <v>1</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G89" s="8"/>
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H89" t="s">
+        <v>46</v>
+      </c>
       <c r="J89" t="s">
-        <v>44</v>
-      </c>
-      <c r="K89" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="O89" s="7">
-        <v>1</v>
-      </c>
-      <c r="P89" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O89" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P89" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
@@ -4024,58 +3993,53 @@
         <v>1</v>
       </c>
       <c r="U89" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y89" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z89" s="8" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B90" s="8">
-        <v>5</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G90" s="8"/>
       <c r="J90" t="s">
         <v>44</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="O90" s="7">
         <v>1</v>
       </c>
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
       <c r="S90" s="1"/>
       <c r="T90">
         <v>1</v>
       </c>
-      <c r="V90" t="s">
-        <v>167</v>
+      <c r="U90" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y90" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z90" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="B91" s="8">
-        <v>4</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D91" s="8"/>
+        <v>5</v>
+      </c>
       <c r="E91" s="8" t="s">
         <v>46</v>
       </c>
@@ -4083,11 +4047,13 @@
         <v>46</v>
       </c>
       <c r="J91" t="s">
-        <v>27</v>
-      </c>
-      <c r="N91" s="1"/>
-      <c r="O91" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="K91" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="O91" s="7">
+        <v>1</v>
       </c>
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
@@ -4096,76 +4062,65 @@
         <v>1</v>
       </c>
       <c r="V91" t="s">
-        <v>14</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B92" s="8">
-        <v>1</v>
-      </c>
-      <c r="C92" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D92" s="8"/>
-      <c r="G92" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J92" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L92" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M92" s="1"/>
+      <c r="E92" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J92" t="s">
+        <v>27</v>
+      </c>
+      <c r="N92" s="1"/>
       <c r="O92" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P92" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
-      <c r="R92" s="1"/>
       <c r="S92" s="1"/>
       <c r="T92">
         <v>1</v>
       </c>
-      <c r="U92" t="s">
-        <v>87</v>
-      </c>
-      <c r="W92" t="s">
-        <v>24</v>
-      </c>
-      <c r="X92" t="s">
-        <v>26</v>
+      <c r="V92" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>155</v>
-      </c>
-      <c r="B93">
-        <v>1</v>
-      </c>
-      <c r="C93" t="s">
-        <v>46</v>
-      </c>
+      <c r="A93" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B93" s="8">
+        <v>1</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
       <c r="G93" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H93" t="s">
-        <v>46</v>
-      </c>
-      <c r="J93" t="s">
-        <v>27</v>
+      <c r="H93" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="L93" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N93" s="1"/>
+      <c r="M93" s="1"/>
       <c r="O93" s="6" t="s">
         <v>31</v>
       </c>
@@ -4173,18 +4128,14 @@
         <v>4</v>
       </c>
       <c r="Q93" s="1"/>
-      <c r="S93" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="R93" s="1"/>
+      <c r="S93" s="1"/>
       <c r="T93">
         <v>1</v>
       </c>
       <c r="U93" t="s">
         <v>87</v>
       </c>
-      <c r="V93" t="s">
-        <v>23</v>
-      </c>
       <c r="W93" t="s">
         <v>24</v>
       </c>
@@ -4194,7 +4145,7 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -4208,13 +4159,13 @@
       <c r="H94" t="s">
         <v>46</v>
       </c>
-      <c r="J94" s="10" t="s">
-        <v>34</v>
+      <c r="J94" t="s">
+        <v>27</v>
       </c>
       <c r="L94" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
       <c r="O94" s="6" t="s">
         <v>31</v>
       </c>
@@ -4222,7 +4173,9 @@
         <v>4</v>
       </c>
       <c r="Q94" s="1"/>
-      <c r="S94" s="1"/>
+      <c r="S94" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T94">
         <v>1</v>
       </c>
@@ -4230,38 +4183,59 @@
         <v>87</v>
       </c>
       <c r="V94" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="W94" t="s">
+        <v>24</v>
+      </c>
+      <c r="X94" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
-      <c r="I95" t="s">
-        <v>46</v>
-      </c>
-      <c r="J95" t="s">
-        <v>44</v>
-      </c>
-      <c r="K95" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="O95" s="7">
-        <v>1</v>
-      </c>
-      <c r="P95" s="1"/>
+      <c r="C95" t="s">
+        <v>46</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H95" t="s">
+        <v>46</v>
+      </c>
+      <c r="J95" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L95" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M95" s="1"/>
+      <c r="O95" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q95" s="1"/>
       <c r="S95" s="1"/>
       <c r="T95">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="U95" t="s">
+        <v>87</v>
+      </c>
+      <c r="V95" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -4273,7 +4247,7 @@
         <v>44</v>
       </c>
       <c r="K96" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O96" s="7">
         <v>1</v>
@@ -4285,10 +4259,36 @@
         <v>0</v>
       </c>
     </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>7</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="I97" t="s">
+        <v>46</v>
+      </c>
+      <c r="J97" t="s">
+        <v>44</v>
+      </c>
+      <c r="K97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O97" s="7">
+        <v>1</v>
+      </c>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Z94" xr:uid="{32A5E267-3EA0-4E71-9FF7-CDD296A6772F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z94">
-      <sortCondition ref="A1:A93"/>
+  <autoFilter ref="A1:Z95" xr:uid="{32A5E267-3EA0-4E71-9FF7-CDD296A6772F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z95">
+      <sortCondition ref="A1:A94"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
JEYZ-81 : Virtual thread analysis support
</commit_message>
<xml_diff>
--- a/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
+++ b/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\jeyzer\jeyzer-analyzer\analyzer\src\main\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3758A7DD-0899-4A79-98F8-68F9E3D217ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03970EDE-B698-486B-88B8-CB6249BFE50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Level colors" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event params logged'!$A$1:$Z$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event params logged'!$A$1:$Z$96</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="206">
   <si>
     <t>END DATE</t>
   </si>
@@ -658,6 +658,12 @@
   </si>
   <si>
     <t>Executor detected</t>
+  </si>
+  <si>
+    <t>Virtual threads CPU consuming</t>
+  </si>
+  <si>
+    <t>Global virtual thread limit</t>
   </si>
 </sst>
 </file>
@@ -1183,13 +1189,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z97"/>
+  <dimension ref="A1:Z99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2414,65 +2420,59 @@
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="8">
-        <v>1</v>
+      <c r="A38" t="s">
+        <v>205</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" t="s">
         <v>46</v>
       </c>
       <c r="J38" t="s">
         <v>27</v>
       </c>
       <c r="N38" s="1"/>
-      <c r="O38" s="7">
-        <v>1</v>
+      <c r="O38" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="S38" s="1"/>
+      <c r="V38" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>154</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
+      <c r="A39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J39" t="s">
         <v>27</v>
       </c>
       <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
+      <c r="O39" s="7">
+        <v>1</v>
+      </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
-      <c r="S39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T39">
-        <v>1</v>
-      </c>
-      <c r="V39" t="s">
-        <v>23</v>
-      </c>
+      <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2487,193 +2487,195 @@
         <v>46</v>
       </c>
       <c r="J40" t="s">
-        <v>34</v>
-      </c>
-      <c r="M40" s="1"/>
-      <c r="O40" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
-      <c r="S40" s="1"/>
+      <c r="S40" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T40">
         <v>1</v>
       </c>
       <c r="V40" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" s="8" t="s">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
         <v>46</v>
       </c>
       <c r="J41" t="s">
-        <v>145</v>
-      </c>
-      <c r="O41" s="7">
-        <v>1</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>146</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M41" s="1"/>
+      <c r="O41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41">
         <v>1</v>
       </c>
+      <c r="V41" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="A42" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J42" t="s">
-        <v>44</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L42" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O42" s="6"/>
+        <v>145</v>
+      </c>
+      <c r="O42" s="7">
+        <v>1</v>
+      </c>
       <c r="P42" s="1" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42">
         <v>1</v>
       </c>
-      <c r="U42" t="s">
-        <v>87</v>
-      </c>
-      <c r="V42" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="8">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43">
         <v>2</v>
       </c>
-      <c r="E43" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F43" s="8" t="s">
+      <c r="G43" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" t="s">
         <v>46</v>
       </c>
       <c r="J43" t="s">
-        <v>27</v>
-      </c>
-      <c r="N43" s="1"/>
-      <c r="O43" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P43" s="1"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43">
         <v>1</v>
       </c>
+      <c r="U43" t="s">
+        <v>87</v>
+      </c>
       <c r="V43" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="8">
         <v>2</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="E44" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J44" t="s">
-        <v>61</v>
-      </c>
-      <c r="L44" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N44" s="1"/>
+      <c r="O44" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O44" s="6"/>
-      <c r="P44" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44">
-        <v>2</v>
-      </c>
-      <c r="U44" t="s">
-        <v>87</v>
+        <v>1</v>
+      </c>
+      <c r="V44" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>46</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
         <v>46</v>
       </c>
       <c r="J45" t="s">
-        <v>27</v>
-      </c>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O45" s="6"/>
+      <c r="P45" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45">
-        <v>1</v>
-      </c>
-      <c r="V45" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="U45" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="8">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46">
         <v>3</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" t="s">
         <v>46</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" t="s">
         <v>46</v>
       </c>
       <c r="J46" t="s">
@@ -2688,147 +2690,144 @@
         <v>1</v>
       </c>
       <c r="V46" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>46</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H47" t="s">
+      <c r="A47" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="8">
+        <v>3</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J47" t="s">
         <v>27</v>
       </c>
-      <c r="L47" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="N47" s="1"/>
-      <c r="O47" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P47" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
       <c r="S47" s="1"/>
       <c r="T47">
         <v>1</v>
       </c>
-      <c r="U47" t="s">
-        <v>87</v>
-      </c>
       <c r="V47" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H48" t="s">
+        <v>46</v>
+      </c>
+      <c r="J48" t="s">
+        <v>27</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N48" s="1"/>
+      <c r="O48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="U48" t="s">
+        <v>87</v>
+      </c>
+      <c r="V48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>168</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>3</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" t="s">
-        <v>46</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="E49" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" t="s">
+        <v>46</v>
+      </c>
+      <c r="J49" t="s">
         <v>51</v>
       </c>
-      <c r="K48" s="6" t="s">
+      <c r="K49" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="S48" s="1"/>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B49" s="8">
-        <v>2</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J49" t="s">
-        <v>114</v>
-      </c>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="S49" s="1"/>
-      <c r="T49">
-        <v>1</v>
-      </c>
-      <c r="U49" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B50" s="8">
-        <v>1</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D50" s="8"/>
+        <v>2</v>
+      </c>
       <c r="E50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J50" t="s">
-        <v>27</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
+      <c r="O50" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q50" s="1"/>
-      <c r="S50" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S50" s="1"/>
       <c r="T50">
-        <v>2</v>
-      </c>
-      <c r="V50" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="U50" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="B51" s="8">
         <v>1</v>
@@ -2843,78 +2842,73 @@
       <c r="F51" t="s">
         <v>46</v>
       </c>
-      <c r="J51" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M51" s="1"/>
-      <c r="O51" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="J51" t="s">
+        <v>27</v>
+      </c>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
-      <c r="S51" s="1"/>
+      <c r="S51" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V51" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="B52" s="8">
-        <v>4</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J52" t="s">
-        <v>106</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" t="s">
+        <v>46</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M52" s="1"/>
       <c r="O52" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P52" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52">
         <v>1</v>
       </c>
-      <c r="U52" t="s">
-        <v>88</v>
-      </c>
       <c r="V52" t="s">
-        <v>110</v>
-      </c>
-      <c r="W52" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="B53" s="8">
-        <v>3</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J53" t="s">
-        <v>35</v>
-      </c>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="O53" s="6" t="s">
         <v>31</v>
       </c>
@@ -2924,21 +2918,24 @@
       <c r="Q53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U53" t="s">
         <v>88</v>
       </c>
+      <c r="V53" t="s">
+        <v>110</v>
+      </c>
+      <c r="W53" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="B54" s="8">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>46</v>
@@ -2947,17 +2944,28 @@
         <v>46</v>
       </c>
       <c r="J54" t="s">
-        <v>27</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="M54" s="1"/>
       <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
+      <c r="O54" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q54" s="1"/>
       <c r="S54" s="1"/>
+      <c r="T54">
+        <v>2</v>
+      </c>
+      <c r="U54" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B55" s="8">
         <v>2</v>
@@ -2982,36 +2990,32 @@
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>71</v>
+        <v>198</v>
       </c>
       <c r="B56" s="8">
         <v>2</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="C56" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F56" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J56" t="s">
         <v>27</v>
       </c>
       <c r="N56" s="1"/>
-      <c r="O56" s="7">
-        <v>1</v>
-      </c>
+      <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
-      <c r="S56" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T56">
-        <v>1</v>
-      </c>
-      <c r="V56" t="s">
-        <v>23</v>
-      </c>
+      <c r="S56" s="1"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B57" s="8">
         <v>2</v>
@@ -3040,59 +3044,51 @@
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="B58" s="8">
         <v>2</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F58" s="8" t="s">
+      <c r="D58" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J58" t="s">
-        <v>35</v>
-      </c>
-      <c r="M58" s="1"/>
+        <v>27</v>
+      </c>
       <c r="N58" s="1"/>
-      <c r="O58" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P58" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="O58" s="7">
+        <v>1</v>
+      </c>
+      <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
-      <c r="S58" s="1"/>
+      <c r="S58" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T58">
         <v>1</v>
       </c>
-      <c r="U58" t="s">
-        <v>88</v>
+      <c r="V58" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B59" s="8">
-        <v>1</v>
-      </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="G59" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H59" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J59" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J59" t="s">
+        <v>35</v>
       </c>
       <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
       <c r="O59" s="6" t="s">
         <v>31</v>
       </c>
@@ -3100,52 +3096,62 @@
         <v>4</v>
       </c>
       <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U59" t="s">
-        <v>113</v>
-      </c>
-      <c r="V59" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B60" s="8">
         <v>1</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J60" t="s">
-        <v>44</v>
-      </c>
-      <c r="K60" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="O60" s="7">
-        <v>1</v>
-      </c>
-      <c r="P60" s="1"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="G60" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M60" s="1"/>
+      <c r="O60" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
       <c r="S60" s="1"/>
       <c r="T60">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="U60" t="s">
+        <v>113</v>
+      </c>
+      <c r="V60" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="B61" s="8">
         <v>1</v>
       </c>
-      <c r="C61" s="8"/>
       <c r="D61" s="8" t="s">
         <v>46</v>
       </c>
@@ -3153,7 +3159,7 @@
         <v>44</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="O61" s="7">
         <v>1</v>
@@ -3167,7 +3173,7 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B62" s="8">
         <v>1</v>
@@ -3177,25 +3183,24 @@
         <v>46</v>
       </c>
       <c r="J62" t="s">
-        <v>27</v>
-      </c>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O62" s="7">
+        <v>1</v>
+      </c>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-      <c r="S62" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S62" s="1"/>
       <c r="T62">
-        <v>2</v>
-      </c>
-      <c r="V62" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B63" s="8">
         <v>1</v>
@@ -3205,82 +3210,83 @@
         <v>46</v>
       </c>
       <c r="J63" t="s">
-        <v>34</v>
-      </c>
-      <c r="M63" s="1"/>
-      <c r="O63" s="7">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
-      <c r="S63" s="1"/>
+      <c r="S63" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T63">
         <v>2</v>
       </c>
       <c r="V63" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
-        <v>164</v>
+        <v>66</v>
       </c>
       <c r="B64" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J64" t="s">
-        <v>27</v>
-      </c>
-      <c r="N64" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="M64" s="1"/>
       <c r="O64" s="7">
         <v>1</v>
       </c>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="S64" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S64" s="1"/>
       <c r="T64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V64" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B65" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J65" t="s">
-        <v>44</v>
-      </c>
-      <c r="K65" s="6" t="s">
-        <v>80</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N65" s="1"/>
       <c r="O65" s="7">
         <v>1</v>
       </c>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
-      <c r="S65" s="1"/>
+      <c r="S65" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T65">
         <v>1</v>
+      </c>
+      <c r="V65" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B66" s="8">
         <v>1</v>
@@ -3290,9 +3296,11 @@
         <v>46</v>
       </c>
       <c r="J66" t="s">
-        <v>34</v>
-      </c>
-      <c r="M66" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="O66" s="7">
         <v>1</v>
       </c>
@@ -3302,13 +3310,10 @@
       <c r="T66">
         <v>1</v>
       </c>
-      <c r="V66" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B67" s="8">
         <v>1</v>
@@ -3318,27 +3323,25 @@
         <v>46</v>
       </c>
       <c r="J67" t="s">
-        <v>27</v>
-      </c>
-      <c r="N67" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="M67" s="1"/>
       <c r="O67" s="7">
         <v>1</v>
       </c>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
-      <c r="S67" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="S67" s="1"/>
       <c r="T67">
         <v>1</v>
       </c>
       <c r="V67" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="8">
         <v>1</v>
@@ -3348,72 +3351,73 @@
         <v>46</v>
       </c>
       <c r="J68" t="s">
-        <v>34</v>
-      </c>
-      <c r="M68" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N68" s="1"/>
       <c r="O68" s="7">
         <v>1</v>
       </c>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
-      <c r="S68" s="1"/>
+      <c r="S68" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T68">
         <v>1</v>
       </c>
       <c r="V68" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="B69" s="8">
-        <v>4</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F69" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J69" t="s">
-        <v>148</v>
-      </c>
-      <c r="K69" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N69" s="6" t="s">
-        <v>149</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M69" s="1"/>
       <c r="O69" s="7">
         <v>1</v>
       </c>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
       <c r="S69" s="1"/>
+      <c r="T69">
+        <v>1</v>
+      </c>
       <c r="V69" t="s">
-        <v>150</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="B70" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="F70" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J70" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>180</v>
+        <v>53</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="O70" s="7">
         <v>1</v>
@@ -3421,16 +3425,16 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
       <c r="S70" s="1"/>
-      <c r="T70">
-        <v>1</v>
+      <c r="V70" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B71" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>46</v>
@@ -3442,7 +3446,7 @@
         <v>44</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="O71" s="7">
         <v>1</v>
@@ -3456,10 +3460,10 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B72" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>46</v>
@@ -3468,9 +3472,11 @@
         <v>46</v>
       </c>
       <c r="J72" t="s">
-        <v>34</v>
-      </c>
-      <c r="M72" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>177</v>
+      </c>
       <c r="O72" s="7">
         <v>1</v>
       </c>
@@ -3480,13 +3486,10 @@
       <c r="T72">
         <v>1</v>
       </c>
-      <c r="U72" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B73" s="8">
         <v>1</v>
@@ -3516,7 +3519,7 @@
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B74" s="8">
         <v>1</v>
@@ -3528,11 +3531,9 @@
         <v>46</v>
       </c>
       <c r="J74" t="s">
-        <v>44</v>
-      </c>
-      <c r="K74" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M74" s="1"/>
       <c r="O74" s="7">
         <v>1</v>
       </c>
@@ -3548,7 +3549,7 @@
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B75" s="8">
         <v>1</v>
@@ -3563,7 +3564,7 @@
         <v>44</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O75" s="7">
         <v>1</v>
@@ -3574,13 +3575,16 @@
       <c r="T75">
         <v>1</v>
       </c>
+      <c r="U75" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B76" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>46</v>
@@ -3592,7 +3596,7 @@
         <v>44</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O76" s="7">
         <v>1</v>
@@ -3606,10 +3610,10 @@
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B77" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>46</v>
@@ -3618,9 +3622,11 @@
         <v>46</v>
       </c>
       <c r="J77" t="s">
-        <v>34</v>
-      </c>
-      <c r="M77" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="O77" s="7">
         <v>1</v>
       </c>
@@ -3630,13 +3636,10 @@
       <c r="T77">
         <v>1</v>
       </c>
-      <c r="U77" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B78" s="8">
         <v>1</v>
@@ -3666,7 +3669,7 @@
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B79" s="8">
         <v>1</v>
@@ -3678,11 +3681,9 @@
         <v>46</v>
       </c>
       <c r="J79" t="s">
-        <v>44</v>
-      </c>
-      <c r="K79" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M79" s="1"/>
       <c r="O79" s="7">
         <v>1</v>
       </c>
@@ -3698,7 +3699,7 @@
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B80" s="8">
         <v>1</v>
@@ -3713,7 +3714,7 @@
         <v>44</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="O80" s="7">
         <v>1</v>
@@ -3724,13 +3725,16 @@
       <c r="T80">
         <v>1</v>
       </c>
+      <c r="U80" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B81" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>46</v>
@@ -3742,7 +3746,7 @@
         <v>44</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O81" s="7">
         <v>1</v>
@@ -3756,23 +3760,26 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="B82" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D82" s="8"/>
-      <c r="F82" s="8" t="s">
+      <c r="D82" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J82" t="s">
-        <v>27</v>
-      </c>
-      <c r="N82" s="1"/>
-      <c r="O82"/>
+        <v>44</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="O82" s="7">
+        <v>1</v>
+      </c>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
       <c r="S82" s="1"/>
@@ -3782,241 +3789,236 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="B83" s="8">
-        <v>5</v>
-      </c>
-      <c r="D83" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D83" s="8"/>
+      <c r="F83" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J83" t="s">
-        <v>197</v>
-      </c>
-      <c r="K83" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="O83" s="7">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="N83" s="1"/>
+      <c r="O83"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
       <c r="S83" s="1"/>
-      <c r="U83" t="s">
-        <v>88</v>
+      <c r="T83">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B84" s="8">
-        <v>1</v>
-      </c>
-      <c r="C84" s="8"/>
+        <v>5</v>
+      </c>
       <c r="D84" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J84" t="s">
-        <v>27</v>
-      </c>
-      <c r="N84" s="1"/>
-      <c r="O84"/>
+        <v>197</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="O84" s="7">
+        <v>1</v>
+      </c>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
-      <c r="S84" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T84">
-        <v>1</v>
-      </c>
+      <c r="S84" s="1"/>
       <c r="U84" t="s">
-        <v>190</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="B85" s="8">
-        <v>2</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F85" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J85" t="s">
         <v>27</v>
       </c>
       <c r="N85" s="1"/>
-      <c r="O85" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="O85"/>
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
-      <c r="S85" s="1"/>
+      <c r="S85" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T85">
         <v>1</v>
       </c>
-      <c r="V85" t="s">
-        <v>63</v>
+      <c r="U85" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="B86" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D86" s="8"/>
+      <c r="E86" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="F86" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J86" t="s">
-        <v>44</v>
-      </c>
-      <c r="K86" s="6" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="N86" s="1"/>
-      <c r="O86" s="7">
-        <v>1</v>
+      <c r="O86" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
       <c r="S86" s="1"/>
-      <c r="W86" t="s">
+      <c r="T86">
+        <v>1</v>
+      </c>
+      <c r="V86" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B87" s="8">
+        <v>4</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D87" s="8"/>
+      <c r="F87" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J87" t="s">
+        <v>44</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N87" s="1"/>
+      <c r="O87" s="7">
+        <v>1</v>
+      </c>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="S87" s="1"/>
+      <c r="W87" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>156</v>
       </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F87" t="s">
-        <v>46</v>
-      </c>
-      <c r="J87" s="10" t="s">
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F88" t="s">
+        <v>46</v>
+      </c>
+      <c r="J88" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M87" s="1"/>
-      <c r="O87" s="6" t="s">
+      <c r="M88" s="1"/>
+      <c r="O88" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P87" s="2"/>
-      <c r="Q87" t="s">
+      <c r="P88" s="2"/>
+      <c r="Q88" t="s">
         <v>3</v>
       </c>
-      <c r="S87" s="1"/>
-      <c r="T87">
-        <v>1</v>
-      </c>
-      <c r="U87" t="s">
-        <v>88</v>
-      </c>
-      <c r="V87" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A88" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B88" s="8">
-        <v>1</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E88" s="8"/>
-      <c r="J88" t="s">
-        <v>44</v>
-      </c>
-      <c r="K88" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="O88" s="6"/>
-      <c r="P88" s="2"/>
       <c r="S88" s="1"/>
       <c r="T88">
         <v>1</v>
       </c>
+      <c r="U88" t="s">
+        <v>88</v>
+      </c>
       <c r="V88" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="8">
+        <v>1</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E89" s="8"/>
+      <c r="J89" t="s">
+        <v>44</v>
+      </c>
+      <c r="K89" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89">
-        <v>4</v>
-      </c>
-      <c r="G89" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H89" t="s">
-        <v>46</v>
-      </c>
-      <c r="J89" t="s">
-        <v>27</v>
-      </c>
-      <c r="N89" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O89" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P89" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q89" s="1"/>
-      <c r="R89" s="1"/>
+      <c r="O89" s="6"/>
+      <c r="P89" s="2"/>
       <c r="S89" s="1"/>
       <c r="T89">
         <v>1</v>
       </c>
-      <c r="U89" t="s">
-        <v>87</v>
+      <c r="V89" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A90" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B90" s="8">
-        <v>1</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G90" s="8"/>
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H90" t="s">
+        <v>46</v>
+      </c>
       <c r="J90" t="s">
-        <v>44</v>
-      </c>
-      <c r="K90" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="O90" s="7">
-        <v>1</v>
-      </c>
-      <c r="P90" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N90" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O90" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P90" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
@@ -4024,58 +4026,53 @@
         <v>1</v>
       </c>
       <c r="U90" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y90" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z90" s="8" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B91" s="8">
-        <v>5</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G91" s="8"/>
       <c r="J91" t="s">
         <v>44</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="O91" s="7">
         <v>1</v>
       </c>
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
       <c r="S91" s="1"/>
       <c r="T91">
         <v>1</v>
       </c>
-      <c r="V91" t="s">
-        <v>167</v>
+      <c r="U91" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y91" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z91" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="B92" s="8">
-        <v>4</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D92" s="8"/>
+        <v>5</v>
+      </c>
       <c r="E92" s="8" t="s">
         <v>46</v>
       </c>
@@ -4083,11 +4080,13 @@
         <v>46</v>
       </c>
       <c r="J92" t="s">
-        <v>27</v>
-      </c>
-      <c r="N92" s="1"/>
-      <c r="O92" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="K92" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="O92" s="7">
+        <v>1</v>
       </c>
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
@@ -4096,76 +4095,65 @@
         <v>1</v>
       </c>
       <c r="V92" t="s">
-        <v>14</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B93" s="8">
-        <v>1</v>
-      </c>
-      <c r="C93" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D93" s="8"/>
-      <c r="G93" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H93" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J93" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L93" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M93" s="1"/>
+      <c r="E93" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J93" t="s">
+        <v>27</v>
+      </c>
+      <c r="N93" s="1"/>
       <c r="O93" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P93" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
-      <c r="R93" s="1"/>
       <c r="S93" s="1"/>
       <c r="T93">
         <v>1</v>
       </c>
-      <c r="U93" t="s">
-        <v>87</v>
-      </c>
-      <c r="W93" t="s">
-        <v>24</v>
-      </c>
-      <c r="X93" t="s">
-        <v>26</v>
+      <c r="V93" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>155</v>
-      </c>
-      <c r="B94">
-        <v>1</v>
-      </c>
-      <c r="C94" t="s">
-        <v>46</v>
-      </c>
+      <c r="A94" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B94" s="8">
+        <v>1</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
       <c r="G94" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H94" t="s">
-        <v>46</v>
-      </c>
-      <c r="J94" t="s">
-        <v>27</v>
+      <c r="H94" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J94" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="L94" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N94" s="1"/>
+      <c r="M94" s="1"/>
       <c r="O94" s="6" t="s">
         <v>31</v>
       </c>
@@ -4173,18 +4161,14 @@
         <v>4</v>
       </c>
       <c r="Q94" s="1"/>
-      <c r="S94" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
       <c r="T94">
         <v>1</v>
       </c>
       <c r="U94" t="s">
         <v>87</v>
       </c>
-      <c r="V94" t="s">
-        <v>23</v>
-      </c>
       <c r="W94" t="s">
         <v>24</v>
       </c>
@@ -4194,7 +4178,7 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -4208,13 +4192,13 @@
       <c r="H95" t="s">
         <v>46</v>
       </c>
-      <c r="J95" s="10" t="s">
-        <v>34</v>
+      <c r="J95" t="s">
+        <v>27</v>
       </c>
       <c r="L95" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
       <c r="O95" s="6" t="s">
         <v>31</v>
       </c>
@@ -4222,7 +4206,9 @@
         <v>4</v>
       </c>
       <c r="Q95" s="1"/>
-      <c r="S95" s="1"/>
+      <c r="S95" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="T95">
         <v>1</v>
       </c>
@@ -4230,38 +4216,59 @@
         <v>87</v>
       </c>
       <c r="V95" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="W95" t="s">
+        <v>24</v>
+      </c>
+      <c r="X95" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="B96">
         <v>1</v>
       </c>
-      <c r="I96" t="s">
-        <v>46</v>
-      </c>
-      <c r="J96" t="s">
-        <v>44</v>
-      </c>
-      <c r="K96" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="O96" s="7">
-        <v>1</v>
-      </c>
-      <c r="P96" s="1"/>
+      <c r="C96" t="s">
+        <v>46</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H96" t="s">
+        <v>46</v>
+      </c>
+      <c r="J96" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L96" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M96" s="1"/>
+      <c r="O96" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Q96" s="1"/>
       <c r="S96" s="1"/>
       <c r="T96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="U96" t="s">
+        <v>87</v>
+      </c>
+      <c r="V96" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -4273,7 +4280,7 @@
         <v>44</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O97" s="7">
         <v>1</v>
@@ -4285,10 +4292,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="I98" t="s">
+        <v>46</v>
+      </c>
+      <c r="J98" t="s">
+        <v>44</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O98" s="7">
+        <v>1</v>
+      </c>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="S98" s="1"/>
+      <c r="T98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A99" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B99" s="8">
+        <v>3</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F99" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J99" t="s">
+        <v>27</v>
+      </c>
+      <c r="O99" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="S99" s="1"/>
+      <c r="T99">
+        <v>1</v>
+      </c>
+      <c r="V99" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Z95" xr:uid="{32A5E267-3EA0-4E71-9FF7-CDD296A6772F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z95">
-      <sortCondition ref="A1:A94"/>
+  <autoFilter ref="A1:Z96" xr:uid="{32A5E267-3EA0-4E71-9FF7-CDD296A6772F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z96">
+      <sortCondition ref="A1:A95"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
JEYZ-81 : Virtual thread presence system rule added and process card one removed
</commit_message>
<xml_diff>
--- a/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
+++ b/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\jeyzer\jeyzer-analyzer\analyzer\src\main\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03970EDE-B698-486B-88B8-CB6249BFE50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF97FD0-E80A-4BAF-BC53-1116B8D847A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="208">
   <si>
     <t>END DATE</t>
   </si>
@@ -664,6 +664,12 @@
   </si>
   <si>
     <t>Global virtual thread limit</t>
+  </si>
+  <si>
+    <t>Virtual thread presence</t>
+  </si>
+  <si>
+    <t>virual threads detected</t>
   </si>
 </sst>
 </file>
@@ -1189,13 +1195,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z99"/>
+  <dimension ref="A1:Z100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4350,6 +4356,35 @@
         <v>14</v>
       </c>
     </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A100" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B100" s="8">
+        <v>2</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J100" t="s">
+        <v>44</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="O100" s="7">
+        <v>1</v>
+      </c>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100">
+        <v>0</v>
+      </c>
+      <c r="U100" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Z96" xr:uid="{32A5E267-3EA0-4E71-9FF7-CDD296A6772F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z96">

</xml_diff>

<commit_message>
JEYZ-81 : virtual thread leak rule added
</commit_message>
<xml_diff>
--- a/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
+++ b/analyzer/src/main/doc/monitoring-rules-inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\src\jeyzer\jeyzer-analyzer\analyzer\src\main\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF97FD0-E80A-4BAF-BC53-1116B8D847A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE8FD4A-A7F4-456E-AD08-D71E6836F7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event params logged'!$A$1:$Z$96</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="212">
   <si>
     <t>END DATE</t>
   </si>
@@ -670,6 +671,18 @@
   </si>
   <si>
     <t>virual threads detected</t>
+  </si>
+  <si>
+    <t>Virtual thread leak</t>
+  </si>
+  <si>
+    <t>signal with context</t>
+  </si>
+  <si>
+    <t>unmounted virtual threads still present</t>
+  </si>
+  <si>
+    <t>Must be higher than 8</t>
   </si>
 </sst>
 </file>
@@ -1195,40 +1208,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z100"/>
+  <dimension ref="A1:Z101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A100" sqref="A100"/>
+      <selection pane="bottomRight" activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="13" width="13.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
-    <col min="15" max="15" width="17.109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="24.6640625" customWidth="1"/>
-    <col min="17" max="19" width="13.33203125" customWidth="1"/>
-    <col min="20" max="20" width="12.5546875" customWidth="1"/>
+    <col min="12" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="24.7109375" customWidth="1"/>
+    <col min="17" max="19" width="13.28515625" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" customWidth="1"/>
     <col min="21" max="21" width="21" customWidth="1"/>
-    <col min="22" max="24" width="17.5546875" customWidth="1"/>
-    <col min="25" max="25" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="17.5703125" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1302,7 +1315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>95</v>
       </c>
@@ -1335,7 +1348,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -1368,7 +1381,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -1398,7 +1411,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>140</v>
       </c>
@@ -1426,7 +1439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>141</v>
       </c>
@@ -1452,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>139</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>94</v>
       </c>
@@ -1509,7 +1522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>121</v>
       </c>
@@ -1538,7 +1551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>92</v>
       </c>
@@ -1571,7 +1584,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>93</v>
       </c>
@@ -1610,7 +1623,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>193</v>
       </c>
@@ -1636,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>162</v>
       </c>
@@ -1669,7 +1682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -1711,7 +1724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>100</v>
       </c>
@@ -1737,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1769,7 +1782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>131</v>
       </c>
@@ -1802,7 +1815,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>130</v>
       </c>
@@ -1835,7 +1848,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>134</v>
       </c>
@@ -1864,7 +1877,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>133</v>
       </c>
@@ -1897,7 +1910,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>132</v>
       </c>
@@ -1930,7 +1943,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>136</v>
       </c>
@@ -1960,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>137</v>
       </c>
@@ -1990,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2021,7 +2034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>74</v>
       </c>
@@ -2049,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>202</v>
       </c>
@@ -2077,7 +2090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -2113,7 +2126,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>157</v>
       </c>
@@ -2146,7 +2159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>70</v>
       </c>
@@ -2175,7 +2188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>119</v>
       </c>
@@ -2204,7 +2217,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>89</v>
       </c>
@@ -2237,7 +2250,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>84</v>
       </c>
@@ -2278,7 +2291,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>101</v>
       </c>
@@ -2304,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>191</v>
       </c>
@@ -2328,7 +2341,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2361,7 +2374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>108</v>
       </c>
@@ -2395,7 +2408,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -2425,7 +2438,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>205</v>
       </c>
@@ -2452,7 +2465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>98</v>
       </c>
@@ -2476,7 +2489,7 @@
       <c r="Q39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -2509,7 +2522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>115</v>
       </c>
@@ -2542,7 +2555,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>144</v>
       </c>
@@ -2570,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>118</v>
       </c>
@@ -2609,7 +2622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>91</v>
       </c>
@@ -2639,7 +2652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -2668,7 +2681,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -2699,7 +2712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>72</v>
       </c>
@@ -2730,7 +2743,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -2772,7 +2785,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>168</v>
       </c>
@@ -2798,7 +2811,7 @@
       <c r="Q49" s="1"/>
       <c r="S49" s="1"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>160</v>
       </c>
@@ -2831,7 +2844,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>153</v>
       </c>
@@ -2865,7 +2878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>65</v>
       </c>
@@ -2899,7 +2912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>107</v>
       </c>
@@ -2936,7 +2949,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>159</v>
       </c>
@@ -2969,7 +2982,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>199</v>
       </c>
@@ -2994,7 +3007,7 @@
       <c r="Q55" s="1"/>
       <c r="S55" s="1"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>198</v>
       </c>
@@ -3019,7 +3032,7 @@
       <c r="Q56" s="1"/>
       <c r="S56" s="1"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>71</v>
       </c>
@@ -3048,7 +3061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>120</v>
       </c>
@@ -3077,7 +3090,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>90</v>
       </c>
@@ -3110,7 +3123,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>83</v>
       </c>
@@ -3151,7 +3164,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>102</v>
       </c>
@@ -3177,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>75</v>
       </c>
@@ -3204,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>68</v>
       </c>
@@ -3232,7 +3245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>66</v>
       </c>
@@ -3260,7 +3273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>164</v>
       </c>
@@ -3290,7 +3303,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>79</v>
       </c>
@@ -3317,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>81</v>
       </c>
@@ -3345,7 +3358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>77</v>
       </c>
@@ -3375,7 +3388,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>78</v>
       </c>
@@ -3403,7 +3416,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>147</v>
       </c>
@@ -3435,7 +3448,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>179</v>
       </c>
@@ -3464,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>174</v>
       </c>
@@ -3493,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>178</v>
       </c>
@@ -3523,7 +3536,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>181</v>
       </c>
@@ -3553,7 +3566,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>171</v>
       </c>
@@ -3585,7 +3598,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>173</v>
       </c>
@@ -3614,7 +3627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>172</v>
       </c>
@@ -3643,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>183</v>
       </c>
@@ -3673,7 +3686,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>182</v>
       </c>
@@ -3703,7 +3716,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>186</v>
       </c>
@@ -3735,7 +3748,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>184</v>
       </c>
@@ -3764,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>187</v>
       </c>
@@ -3793,7 +3806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>152</v>
       </c>
@@ -3819,7 +3832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>195</v>
       </c>
@@ -3845,7 +3858,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>189</v>
       </c>
@@ -3873,7 +3886,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>161</v>
       </c>
@@ -3907,7 +3920,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>52</v>
       </c>
@@ -3938,7 +3951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>156</v>
       </c>
@@ -3973,7 +3986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>200</v>
       </c>
@@ -4000,7 +4013,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -4035,7 +4048,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>169</v>
       </c>
@@ -4072,7 +4085,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>165</v>
       </c>
@@ -4104,7 +4117,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>117</v>
       </c>
@@ -4138,7 +4151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>123</v>
       </c>
@@ -4182,7 +4195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>155</v>
       </c>
@@ -4231,7 +4244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>116</v>
       </c>
@@ -4272,7 +4285,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -4298,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -4324,7 +4337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>204</v>
       </c>
@@ -4356,7 +4369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>206</v>
       </c>
@@ -4381,8 +4394,28 @@
       <c r="T100">
         <v>0</v>
       </c>
-      <c r="U100" t="s">
-        <v>88</v>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B101" s="8">
+        <v>4</v>
+      </c>
+      <c r="H101" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J101" t="s">
+        <v>209</v>
+      </c>
+      <c r="K101" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="O101" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="T101">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4404,18 +4437,18 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -4426,7 +4459,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -4434,7 +4467,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -4445,7 +4478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -4456,7 +4489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -4467,7 +4500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -4475,7 +4508,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -4483,7 +4516,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -4491,7 +4524,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
@@ -4499,7 +4532,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -4507,7 +4540,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -4518,7 +4551,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2</v>
       </c>
@@ -4526,7 +4559,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3</v>
       </c>
@@ -4537,7 +4570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>4</v>
       </c>
@@ -4548,7 +4581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>5</v>
       </c>
@@ -4559,7 +4592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>6</v>
       </c>
@@ -4567,7 +4600,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>7</v>
       </c>
@@ -4575,7 +4608,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>8</v>
       </c>
@@ -4583,7 +4616,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>9</v>
       </c>
@@ -4591,7 +4624,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>10</v>
       </c>
@@ -4599,7 +4632,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -4610,7 +4643,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2</v>
       </c>
@@ -4618,7 +4651,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>3</v>
       </c>
@@ -4629,7 +4662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>4</v>
       </c>
@@ -4640,7 +4673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>5</v>
       </c>
@@ -4651,7 +4684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>6</v>
       </c>
@@ -4659,7 +4692,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>7</v>
       </c>
@@ -4667,7 +4700,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>8</v>
       </c>
@@ -4675,7 +4708,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>9</v>
       </c>
@@ -4683,7 +4716,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>10</v>
       </c>

</xml_diff>